<commit_message>
Test cases with 3 new added tests, as well as the given.
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-lab4-ethan-and-oreoluwa-lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD855A85-678C-0D4F-A767-FA0C68848C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD849E-DEC5-4DEE-A1AF-15DABB274FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Test Description</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Green Package 3 months with additional 5 GB data</t>
+  </si>
+  <si>
+    <t>Purple Package 4 months</t>
+  </si>
+  <si>
+    <t>Green Package 4 months with additional 3 GB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue </t>
+  </si>
+  <si>
+    <t>Blue Package 3 months, with additional 2 GB data</t>
   </si>
 </sst>
 </file>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -201,6 +213,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -220,9 +235,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +275,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +381,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,25 +531,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B94F62A-3D0C-2040-8FEF-E1506E31F742}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.875" customWidth="1"/>
+    <col min="6" max="6" width="20.125" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -554,7 +569,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -574,7 +589,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -594,7 +609,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -614,7 +629,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -624,7 +639,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -634,7 +649,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -648,7 +663,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -670,63 +685,169 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="4">
+        <f>C9*C2</f>
+        <v>99.98</v>
+      </c>
+      <c r="G9" s="4">
+        <f>(IF(F9&gt;75,F9-20,0))</f>
+        <v>79.98</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="4">
+        <f>C10*C3</f>
+        <v>140</v>
+      </c>
+      <c r="G10" s="4">
+        <f>C10*C3</f>
+        <v>140</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="4">
+        <f>C11*C4</f>
+        <v>199.9</v>
+      </c>
+      <c r="G11" s="4">
+        <f>C11*C4</f>
+        <v>199.9</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4">
+        <f>C12*C2+(D12*D2)</f>
+        <v>224.97</v>
+      </c>
+      <c r="G12" s="4">
+        <f>(IF(F12&gt;75,F12-20,0))</f>
+        <v>204.97</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+    <row r="13" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4">
+        <f>C4*C13</f>
+        <v>399.8</v>
+      </c>
+      <c r="G13" s="4">
+        <f>C4*C13</f>
+        <v>399.8</v>
+      </c>
       <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10">
+        <f>C14*C2+(D14*D2)</f>
+        <v>244.96</v>
+      </c>
+      <c r="G14" s="4">
+        <f>(IF(F14&gt;75,F14-20,0))</f>
+        <v>224.96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10">
+        <f>C15*C3+(D15*D3)</f>
+        <v>230</v>
+      </c>
+      <c r="G15" s="10">
+        <f>C15*C3+(D15*D3)</f>
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>